<commit_message>
Added instructions, yield calculations and extra-reagents.
</commit_message>
<xml_diff>
--- a/Experimental template.xlsx
+++ b/Experimental template.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\chm-fs.chm.bris.ac.uk\q\vka\oz15314\shareall\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="Settings" sheetId="1" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$N$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$N$27</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>O Zhurakovskyi</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{5AA52D9E-5905-4EF0-A4B3-A0ECF231FBC9}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{8518975B-04AA-4249-9D0B-534B7F826050}">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{D47DB0CA-74D3-41FD-A28F-E65D2AF4C720}">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{E340E3F1-6630-47CB-8BDE-CD398A400032}">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{55E7CC6C-EE11-45C6-BA90-C87775CDD230}">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{59E8B381-F252-4C75-9AC9-09D09436C7C0}">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{1808C2C6-2F4C-48A0-B76D-E0028F233CEF}">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{3452920A-0384-4F7E-A44B-AFBAE654E2B1}">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{77576F36-159B-4F8F-91E2-58BA7C492DEE}">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{84A286E9-C51E-41F8-A9DA-CD7F097BA6C6}">
+    <comment ref="D7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -273,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{0CEDEC90-6DEA-45EE-92C3-3E660B4227A2}">
+    <comment ref="F7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{27B825F4-0912-4A41-AD8D-82473FFB065A}">
+    <comment ref="I7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{15FB7145-6B5E-4725-99FC-F5EB78E04E31}">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{8AC037E7-0F4E-4FB9-B300-98DF38516ECE}">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -369,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{E143374B-2E48-41B6-AECA-E8C0626824F5}">
+    <comment ref="I8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{31CF62A1-9816-4FAD-825E-9EDF4401A892}">
+    <comment ref="D9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -401,7 +397,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>O Zhurakovskyi:</t>
         </r>
@@ -410,7 +406,81 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Automatic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>O Zhurakovskyi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Automatic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>O Zhurakovskyi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Automatic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>O Zhurakovskyi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Automatic based on solvent 1 + solvent 2.</t>
@@ -422,12 +492,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>O Zhurakovskyi</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8695D279-6070-48B2-92B8-024CF0720BB1}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{BCD5FE79-BEF7-40C2-B28F-903483BE39EB}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -480,7 +550,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>volume units</t>
   </si>
@@ -585,16 +655,55 @@
   </si>
   <si>
     <t>This version:</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>1. Go to "Settings" tab and change  the notebook prefix what you like (e.g. your initials).</t>
+  </si>
+  <si>
+    <t>2. Save the file on disk.</t>
+  </si>
+  <si>
+    <t>3. Copy the Template into a new tab (right-click "Template" -&gt; Move or Copy... -&gt; Create a Copy -&gt; OK</t>
+  </si>
+  <si>
+    <t>4. Rename the copied tab with your experiment number (e.g. 001). The spreadsheet will automatically change the contents of the title cell.</t>
+  </si>
+  <si>
+    <t>5. Double-click the ChemDraw scheme and change it to your reaction.</t>
+  </si>
+  <si>
+    <t>Reagent 5</t>
+  </si>
+  <si>
+    <t>Solvent 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yield = </t>
+  </si>
+  <si>
+    <t>6. Fill the bolded cells as appropriate</t>
+  </si>
+  <si>
+    <t>7. Unbolded cells should auto-fill</t>
+  </si>
+  <si>
+    <t>8. You can choose between g and mg for weights, and uL/mL for volumes. The calculations will adjust automatically</t>
+  </si>
+  <si>
+    <t>9. The yield will be calculated automatically , taking g/mg and %purity into account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,14 +768,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <u/>
@@ -674,6 +785,15 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -691,7 +811,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -960,6 +1080,33 @@
         <color indexed="64"/>
       </top>
       <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -969,7 +1116,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -978,9 +1125,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -993,22 +1137,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -1016,12 +1148,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1060,9 +1186,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1070,12 +1193,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1097,94 +1214,192 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1204,81 +1419,21 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>447675</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>200025</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>352425</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:A3" totalsRowShown="0">
-  <autoFilter ref="A1:A3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="volume units"/>
+    <tableColumn id="1" name="volume units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B1:B3" totalsRowShown="0">
-  <autoFilter ref="B1:B3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="B1:B3" totalsRowShown="0">
+  <autoFilter ref="B1:B3"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="mass units"/>
+    <tableColumn id="1" name="mass units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1327,7 +1482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1362,7 +1517,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1539,26 +1694,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" customWidth="1"/>
@@ -1571,59 +1726,59 @@
     <col min="14" max="14" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="71" t="str">
+    <row r="1" spans="1:14" ht="27.75" customHeight="1">
+      <c r="E1" s="61" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>OZ-Template</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="78" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="72" t="s">
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="72"/>
-    </row>
-    <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-    </row>
-    <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="N1" s="62"/>
+    </row>
+    <row r="2" spans="1:14" ht="27.75" customHeight="1">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+    </row>
+    <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1">
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="35"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1650,28 +1805,30 @@
       <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="76"/>
-      <c r="N4" s="77"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="40" t="s">
+      <c r="M4" s="66"/>
+      <c r="N4" s="67"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1">
+      <c r="A5" s="40">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="92">
         <v>1</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="27">
         <f>IF(E5="mg",H5*I5/IF(K5&gt;0,K5,1),H5*I5/IF(K5&gt;0,K5,1)/1000)</f>
         <v>1.9959183673469387</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f>IF(J5&gt;0,
        IF(G5="uL",
             IF(K5&gt;0, H5*I5/K5/J5, H5*I5/J5),
@@ -1681,44 +1838,46 @@
 )</f>
         <v>1.6359986617597861</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="92">
         <v>163</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="105">
         <v>12</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="92">
         <v>1.22</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="97">
         <v>0.98</v>
       </c>
-      <c r="L5" s="73" t="s">
+      <c r="L5" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="41" t="s">
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1">
+      <c r="A6" s="39">
+        <v>2</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>1.2</v>
       </c>
-      <c r="D6" s="20">
-        <f t="shared" ref="D6:D8" si="0">IF(E6="mg",H6*I6/IF(K6&gt;0,K6,1),H6*I6/IF(K6&gt;0,K6,1)/1000)</f>
+      <c r="D6" s="13">
+        <f>IF(E6="mg",H6*I6/IF(K6&gt;0,K6,1),H6*I6/IF(K6&gt;0,K6,1)/1000)</f>
         <v>1324.8</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="11" t="str">
-        <f t="shared" ref="F6:F8" si="1">IF(J6&gt;0,
+      <c r="F6" s="9" t="str">
+        <f t="shared" ref="F6:F9" si="0">IF(J6&gt;0,
        IF(G6="uL",
             IF(K6&gt;0, H6*I6/K6/J6, H6*I6/J6),
             IF(K6&gt;0, H6*I6/K6/J6/1000, H6*I6/J6/1000)
@@ -1727,188 +1886,280 @@
 )</f>
         <v/>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="93">
         <v>92</v>
       </c>
-      <c r="I6" s="9">
-        <f>I5*C6/C5</f>
+      <c r="I6" s="106">
+        <f>$I$5*C6/$C$5</f>
         <v>14.399999999999999</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="63"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="26" t="s">
+      <c r="J6" s="93"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="53"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="38">
+        <v>3</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="20">
-        <f t="shared" ref="D7" si="2">IF(E7="mg",H7*I7/IF(K7&gt;0,K7,1),H7*I7/IF(K7&gt;0,K7,1)/1000)</f>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13">
+        <f t="shared" ref="D7:D8" si="1">IF(E7="mg",H7*I7/IF(K7&gt;0,K7,1),H7*I7/IF(K7&gt;0,K7,1)/1000)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="11" t="str">
+      <c r="F7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="94">
+        <v>150</v>
+      </c>
+      <c r="I7" s="106">
+        <f t="shared" ref="I7:I8" si="2">$I$5*C7/$C$5</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="102"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="56"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="71">
+        <v>4</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="9" t="str">
+        <f t="shared" ref="F8" si="3">IF(J8&gt;0,
+       IF(G8="uL",
+            IF(K8&gt;0, H8*I8/K8/J8, H8*I8/J8),
+            IF(K8&gt;0, H8*I8/K8/J8/1000, H8*I8/J8/1000)
+       ),
+""
+)</f>
         <v/>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H8" s="94">
         <v>150</v>
       </c>
-      <c r="I7" s="13">
-        <f>C7/C5*I5</f>
+      <c r="I8" s="106">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="66"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24">
+      <c r="J8" s="103"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="46"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="36">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17">
+        <f t="shared" ref="D6:D9" si="4">IF(E9="mg",H9*I9/IF(K9&gt;0,K9,1),H9*I9/IF(K9&gt;0,K9,1)/1000)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="94">
+        <v>150</v>
+      </c>
+      <c r="I9" s="106">
+        <f>$I$5*C9/$C$5</f>
         <v>0</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="26">
-        <v>150</v>
-      </c>
-      <c r="I8" s="13">
-        <f>C8/C5*I5</f>
+      <c r="J9" s="104"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="56"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="37"/>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="95">
+        <v>7</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="77">
+        <f>I5/(SUM(D10:D12))</f>
+        <v>1.7142857142857142</v>
+      </c>
+      <c r="J10" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="26"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="58"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="71"/>
+      <c r="B11" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="96">
         <v>0</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="66"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4">
-        <v>7</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="E11" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="60">
-        <f>I5/(D9+D10)</f>
-        <v>1.7142857142857142</v>
-      </c>
-      <c r="J9" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="33"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="68"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23">
+      <c r="F11" s="73"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="76"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="36"/>
+      <c r="B12" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="96">
         <v>0</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="70"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="43" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="60"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="37"/>
+      <c r="B13" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="30">
-        <f>IF(E11="mg",H11*I11,H11*I11/1000)</f>
+      <c r="D13" s="23">
+        <f>IF(E13="mg",H13*I13,H13*I13/1000)</f>
         <v>1296</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="29">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="33">
         <v>108</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I13" s="23">
         <f>I5</f>
         <v>12</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="56"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15" t="s">
+      <c r="J13" s="22"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="50"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="71"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="54"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="D14" s="107">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="88"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A15" s="34"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="91">
+        <f>IF(E13=E14,D14*IF(K14&gt;0,K14,1)/D13, IF(AND(E14="mg",E13="g"),D14*IF(K14&gt;0,K14,1)/D13/1000, IF(AND(E14="g",E13="mg"),D14*IF(K14&gt;0,K14,1)/D13*1000)))</f>
+        <v>0.77160493827160492</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="48"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1918,61 +2169,36 @@
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L13:N13"/>
     <mergeCell ref="A2:N3"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="I10:I12"/>
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L8:N8"/>
     <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L12:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
   <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="ChemDraw.Document.6.0" shapeId="1025" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>447675</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>200025</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>352425</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="ChemDraw.Document.6.0" shapeId="1025" r:id="rId4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <oleObject progId="ChemDraw.Document.6.0" shapeId="1025" r:id="rId3"/>
   </oleObjects>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Settings!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E11 E5:E8</xm:sqref>
+          <xm:sqref>E13 E5:E9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Settings!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:E10 G5:G9</xm:sqref>
+          <xm:sqref>E10:E12 G5:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1981,14 +2207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -1996,62 +2222,62 @@
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="41" t="s">
         <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="81">
-        <v>43146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="E3" s="43">
+        <v>43233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:5">
+      <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6F417607-8C1D-47F8-9B48-875554E31BED}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -2061,4 +2287,109 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="92.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.75">
+      <c r="A1" s="69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30">
+      <c r="A6" s="70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="30">
+      <c r="A10" s="70" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="70"/>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="70"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="70"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="70"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="70"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="70"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="70"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="70"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="70"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="70"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="70"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="70"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>